<commit_message>
excitation cage table mount H25 mm model for 3D print
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Telecentric_Lens_Overview.xlsx
+++ b/Benchtop/parts-list/Telecentric_Lens_Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop-v2\parts-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5678C77-7F2E-4F5D-BE4F-E9B659567E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77D87ED-3704-424C-821D-8FEBA0A8445D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Magnification</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>10'000 EUR</t>
+  </si>
+  <si>
+    <t>Olympus XLFluor 4x / 340 NA 0.28</t>
+  </si>
+  <si>
+    <t>Olympus</t>
+  </si>
+  <si>
+    <t>M34x1</t>
   </si>
 </sst>
 </file>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:M20"/>
+  <dimension ref="A3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +663,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G20" si="0">0.5/(2*F4)</f>
+        <f t="shared" ref="G4:G21" si="0">0.5/(2*F4)</f>
         <v>33.783783783783782</v>
       </c>
       <c r="H4" s="2">
@@ -850,15 +859,15 @@
         <v>6.0975609756097562</v>
       </c>
       <c r="H9" s="7">
-        <f t="shared" ref="H9:H20" si="16">12.61/A9</f>
+        <f t="shared" ref="H9:H21" si="16">12.61/A9</f>
         <v>25.22</v>
       </c>
       <c r="I9" s="7">
-        <f t="shared" ref="I9:I20" si="17">21.49/A9</f>
+        <f t="shared" ref="I9:I21" si="17">21.49/A9</f>
         <v>42.98</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" ref="J9:J20" si="18">4.25/A9</f>
+        <f t="shared" ref="J9:J21" si="18">4.25/A9</f>
         <v>8.5</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1283,6 +1292,45 @@
       <c r="J20" s="2">
         <f t="shared" si="18"/>
         <v>1.4166666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.89285714285714279</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="16"/>
+        <v>3.1524999999999999</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="17"/>
+        <v>5.3724999999999996</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="18"/>
+        <v>1.0625</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1300,8 +1348,9 @@
     <hyperlink ref="B6" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B4" r:id="rId12" display="https://www.edmundoptics.com/p/0179x-35mm-f-mount-titantl-telecentric-lens/38722/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B21" r:id="rId14" xr:uid="{9F3CB3DB-A9D8-4F4B-82A3-F2B7FF5C7500}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3D model legs w 5 mm offset; objectives list update
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Telecentric_Lens_Overview.xlsx
+++ b/Benchtop/parts-list/Telecentric_Lens_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61B864E-BEBC-4AA4-814E-F34690A04B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C572107-FEA6-4344-B929-9AB876CF2DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
-  <si>
-    <t>Magnification</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
   <si>
     <t>Product Name</t>
   </si>
@@ -210,17 +207,92 @@
     <t>1200 EUR</t>
   </si>
   <si>
-    <t>M25 x 0.75</t>
-  </si>
-  <si>
-    <t>Not tested</t>
+    <t>TL4X-SAP</t>
+  </si>
+  <si>
+    <t>1958 EUR</t>
+  </si>
+  <si>
+    <t>Tested, very good</t>
+  </si>
+  <si>
+    <t>C-Mount, M25 x 0.75</t>
+  </si>
+  <si>
+    <t>C-mount, M25 x 0.75</t>
+  </si>
+  <si>
+    <t>Plan Apo</t>
+  </si>
+  <si>
+    <t>869 EUR</t>
+  </si>
+  <si>
+    <t>M40 x 36 TPI</t>
+  </si>
+  <si>
+    <t>797 EUR</t>
+  </si>
+  <si>
+    <t>Nyquist sampling</t>
+  </si>
+  <si>
+    <t>Undersampling</t>
+  </si>
+  <si>
+    <t>1467 EUR</t>
+  </si>
+  <si>
+    <t>882 EUR</t>
+  </si>
+  <si>
+    <t>M26 x 36 TPI</t>
+  </si>
+  <si>
+    <t>666 EUR</t>
+  </si>
+  <si>
+    <t>4469 EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Apo Brightfield and Darkfield </t>
+  </si>
+  <si>
+    <t>Plan Apo HR</t>
+  </si>
+  <si>
+    <t>4000 EUR?</t>
+  </si>
+  <si>
+    <t>1265 EUR</t>
+  </si>
+  <si>
+    <t>Mag.</t>
+  </si>
+  <si>
+    <t>M PL APO MACRO</t>
+  </si>
+  <si>
+    <t>Leica</t>
+  </si>
+  <si>
+    <t>3000? EUR</t>
+  </si>
+  <si>
+    <t>Near-Nyquist sampling</t>
+  </si>
+  <si>
+    <t>M32</t>
+  </si>
+  <si>
+    <t>Mitutoyo/Edmund</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,8 +341,24 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +373,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -303,7 +409,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -319,16 +425,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -612,63 +734,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:M22"/>
+  <dimension ref="A3:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
     <col min="6" max="6" width="8.21875" customWidth="1"/>
-    <col min="7" max="7" width="14" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14" style="16" customWidth="1"/>
     <col min="8" max="8" width="9.109375" style="2"/>
     <col min="9" max="9" width="11.44140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="I3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="8"/>
     </row>
@@ -677,13 +799,13 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
       </c>
       <c r="E4">
         <v>351</v>
@@ -691,8 +813,8 @@
       <c r="F4">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G22" si="0">0.5/(2*F4)</f>
+      <c r="G4" s="16">
+        <f t="shared" ref="G4:G32" si="0">0.5/(2*F4)</f>
         <v>33.783783783783782</v>
       </c>
       <c r="H4" s="2">
@@ -708,7 +830,7 @@
         <v>23.743016759776538</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -716,13 +838,13 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
       </c>
       <c r="E5">
         <v>267</v>
@@ -730,7 +852,7 @@
       <c r="F5">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
         <v>33.783783783783782</v>
       </c>
@@ -747,7 +869,7 @@
         <v>17.857142857142858</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -755,13 +877,13 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
       </c>
       <c r="E6">
         <v>182</v>
@@ -769,7 +891,7 @@
       <c r="F6">
         <v>2.3E-2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="16">
         <f t="shared" si="0"/>
         <v>10.869565217391305</v>
       </c>
@@ -786,7 +908,7 @@
         <v>15.178571428571427</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -794,13 +916,13 @@
         <v>0.33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7">
         <v>347</v>
@@ -808,7 +930,7 @@
       <c r="F7">
         <v>0.02</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="16">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
@@ -825,7 +947,7 @@
         <v>12.878787878787879</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -833,13 +955,13 @@
         <v>0.35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>213</v>
@@ -847,582 +969,1012 @@
       <c r="F8">
         <v>2.3E-2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="16">
         <f t="shared" si="0"/>
         <v>10.869565217391305</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" ref="H8" si="13">12.61/A8</f>
+        <f t="shared" ref="H8:H9" si="13">12.61/A8</f>
         <v>36.028571428571432</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" ref="I8" si="14">21.49/A8</f>
+        <f t="shared" ref="I8:I9" si="14">21.49/A8</f>
         <v>61.4</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" ref="J8" si="15">4.25/A8</f>
+        <f t="shared" ref="J8:J9" si="15">4.25/A8</f>
         <v>12.142857142857144</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9">
+        <v>0.4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G9" s="16">
+        <f t="shared" si="0"/>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="13"/>
+        <v>31.524999999999999</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="14"/>
+        <v>53.724999999999994</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="15"/>
+        <v>10.625</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <v>0.5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6">
         <v>175</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F10" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>6.0975609756097562</v>
       </c>
-      <c r="H9" s="7">
-        <f t="shared" ref="H9:H22" si="16">12.61/A9</f>
+      <c r="H10" s="7">
+        <f t="shared" ref="H10:H32" si="16">12.61/A10</f>
         <v>25.22</v>
       </c>
-      <c r="I9" s="7">
-        <f t="shared" ref="I9:I22" si="17">21.49/A9</f>
+      <c r="I10" s="7">
+        <f t="shared" ref="I10:I32" si="17">21.49/A10</f>
         <v>42.98</v>
       </c>
-      <c r="J9" s="7">
-        <f t="shared" ref="J9:J22" si="18">4.25/A9</f>
+      <c r="J10" s="7">
+        <f t="shared" ref="J10:J32" si="18">4.25/A10</f>
         <v>8.5</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0.6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10">
-        <v>132</v>
-      </c>
-      <c r="F10">
-        <v>0.08</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>3.125</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" ref="H10" si="19">12.61/A10</f>
-        <v>21.016666666666666</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" ref="I10" si="20">21.49/A10</f>
-        <v>35.816666666666663</v>
-      </c>
-      <c r="J10" s="2">
-        <f t="shared" ref="J10" si="21">4.25/A10</f>
-        <v>7.0833333333333339</v>
-      </c>
+      <c r="K10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0.82</v>
+        <v>0.6</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>270</v>
+        <v>132</v>
       </c>
       <c r="F11">
-        <v>0.66</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.37878787878787878</v>
+        <v>0.08</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" si="0"/>
+        <v>3.125</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" ref="H11" si="22">12.61/A11</f>
-        <v>15.378048780487806</v>
+        <f t="shared" ref="H11" si="19">12.61/A11</f>
+        <v>21.016666666666666</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" ref="I11" si="23">21.49/A11</f>
-        <v>26.207317073170731</v>
+        <f t="shared" ref="I11" si="20">21.49/A11</f>
+        <v>35.816666666666663</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" ref="J11" si="24">4.25/A11</f>
-        <v>5.1829268292682933</v>
+        <f t="shared" ref="J11" si="21">4.25/A11</f>
+        <v>7.0833333333333339</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
+        <v>0.82</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>270</v>
+      </c>
+      <c r="F12">
+        <v>0.66</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="shared" si="0"/>
+        <v>0.37878787878787878</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" ref="H12" si="22">12.61/A12</f>
+        <v>15.378048780487806</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" ref="I12" si="23">21.49/A12</f>
+        <v>26.207317073170731</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" ref="J12" si="24">4.25/A12</f>
+        <v>5.1829268292682933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>0.92</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12">
+      <c r="E13">
         <v>170</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="16">
         <f t="shared" si="0"/>
         <v>3.6231884057971011</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <f t="shared" si="16"/>
         <v>13.706521739130434</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I13" s="2">
         <f t="shared" si="17"/>
         <v>23.35869565217391</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J13" s="2">
         <f t="shared" si="18"/>
         <v>4.6195652173913038</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>0.9</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="4">
         <v>111</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F14" s="4">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G14" s="18">
         <f t="shared" si="0"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H14" s="5">
         <f t="shared" si="16"/>
         <v>14.011111111111109</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I14" s="5">
         <f t="shared" si="17"/>
         <v>23.877777777777776</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J14" s="5">
         <f t="shared" si="18"/>
         <v>4.7222222222222223</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="K14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14">
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
         <v>157</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="16">
         <f t="shared" si="0"/>
         <v>3.5211267605633805</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H15" s="2">
         <f t="shared" si="16"/>
         <v>12.61</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I15" s="2">
         <f t="shared" si="17"/>
         <v>21.49</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J15" s="2">
         <f t="shared" si="18"/>
         <v>4.25</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+    <row r="16" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>1</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="8">
+        <v>60</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="16"/>
+        <v>12.61</v>
+      </c>
+      <c r="I16" s="9">
+        <f t="shared" si="17"/>
+        <v>21.49</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="18"/>
+        <v>4.25</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>1.2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4">
         <v>155</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F17" s="4">
         <v>0.08</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G17" s="18">
         <f t="shared" si="0"/>
         <v>3.125</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H17" s="5">
         <f t="shared" si="16"/>
         <v>10.508333333333333</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I17" s="5">
         <f t="shared" si="17"/>
         <v>17.908333333333331</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J17" s="5">
         <f t="shared" si="18"/>
         <v>3.541666666666667</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="K17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>1.3</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16">
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18">
         <v>110</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G18" s="16">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H18" s="2">
         <f t="shared" si="16"/>
         <v>9.6999999999999993</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I18" s="2">
         <f t="shared" si="17"/>
         <v>16.530769230769231</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J18" s="2">
         <f t="shared" si="18"/>
         <v>3.2692307692307692</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>1.5</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17">
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19">
         <v>100</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G19" s="16">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H19" s="2">
         <f t="shared" si="16"/>
         <v>8.4066666666666663</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I19" s="2">
         <f t="shared" si="17"/>
         <v>14.326666666666666</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J19" s="2">
         <f t="shared" si="18"/>
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18">
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20">
         <v>50</v>
       </c>
-      <c r="F18">
+      <c r="F20">
         <v>0.112</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G20" s="16">
         <f t="shared" si="0"/>
         <v>2.2321428571428572</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H20" s="2">
         <f t="shared" si="16"/>
         <v>6.3049999999999997</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I20" s="2">
         <f t="shared" si="17"/>
         <v>10.744999999999999</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J20" s="2">
         <f t="shared" si="18"/>
         <v>2.125</v>
       </c>
-      <c r="L18" t="s">
-        <v>15</v>
-      </c>
-      <c r="M18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
+      <c r="L20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="B21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="12">
         <v>75</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F21" s="12">
         <v>0.1</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G21" s="19">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H21" s="13">
         <f t="shared" si="16"/>
         <v>6.3049999999999997</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I21" s="13">
         <f t="shared" si="17"/>
         <v>10.744999999999999</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J21" s="13">
         <f t="shared" si="18"/>
         <v>2.125</v>
       </c>
-      <c r="K19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12">
+      <c r="K21" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21">
         <v>2</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B22" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="D22" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="13">
+      <c r="E22" s="23">
         <v>56.3</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F22" s="23">
         <v>0.1</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G22" s="28">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H22" s="24">
         <f t="shared" si="16"/>
         <v>6.3049999999999997</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I22" s="24">
         <f t="shared" si="17"/>
         <v>10.744999999999999</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J22" s="24">
         <f t="shared" si="18"/>
         <v>2.125</v>
       </c>
-      <c r="K20" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="L20" s="13" t="s">
+      <c r="K22" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="L22" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="23" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <v>2</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="27">
+        <v>34</v>
+      </c>
+      <c r="F23" s="27">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G23" s="28">
+        <f t="shared" si="0"/>
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="H23" s="29">
+        <f t="shared" si="16"/>
+        <v>6.3049999999999997</v>
+      </c>
+      <c r="I23" s="29">
+        <f t="shared" si="17"/>
+        <v>10.744999999999999</v>
+      </c>
+      <c r="J23" s="29">
+        <f t="shared" si="18"/>
+        <v>2.125</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="M23" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
+        <v>2</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="12">
+        <v>34</v>
+      </c>
+      <c r="F24" s="12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G24" s="19">
+        <f t="shared" si="0"/>
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="H24" s="13">
+        <f t="shared" si="16"/>
+        <v>6.3049999999999997</v>
+      </c>
+      <c r="I24" s="13">
+        <f t="shared" si="17"/>
+        <v>10.744999999999999</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" si="18"/>
+        <v>2.125</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>3</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25">
         <v>78</v>
       </c>
-      <c r="F21">
+      <c r="F25">
         <v>0.1</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G25" s="16">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H25" s="2">
         <f t="shared" si="16"/>
         <v>4.2033333333333331</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I25" s="2">
         <f t="shared" si="17"/>
         <v>7.1633333333333331</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J25" s="2">
         <f t="shared" si="18"/>
         <v>1.4166666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="26" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
         <v>4</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22">
-        <v>30</v>
-      </c>
-      <c r="F22">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.89285714285714279</v>
-      </c>
-      <c r="H22" s="2">
+      <c r="B26" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="30">
+        <v>17</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="15">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="H26" s="9">
         <f t="shared" si="16"/>
         <v>3.1524999999999999</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I26" s="9">
         <f t="shared" si="17"/>
         <v>5.3724999999999996</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J26" s="9">
         <f t="shared" si="18"/>
         <v>1.0625</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>54</v>
+      <c r="K26" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>4</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="8">
+        <v>30</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G27" s="15">
+        <f t="shared" si="0"/>
+        <v>0.89285714285714279</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="16"/>
+        <v>3.1524999999999999</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" si="17"/>
+        <v>5.3724999999999996</v>
+      </c>
+      <c r="J27" s="9">
+        <f t="shared" si="18"/>
+        <v>1.0625</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>5</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="8">
+        <v>34</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G28" s="15">
+        <f t="shared" si="0"/>
+        <v>1.7857142857142856</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="16"/>
+        <v>2.5219999999999998</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="shared" si="17"/>
+        <v>4.298</v>
+      </c>
+      <c r="J28" s="9">
+        <f t="shared" si="18"/>
+        <v>0.85</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29">
+        <v>34</v>
+      </c>
+      <c r="F29">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G29" s="16">
+        <f t="shared" si="0"/>
+        <v>1.7857142857142856</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="16"/>
+        <v>2.5219999999999998</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="17"/>
+        <v>4.298</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="18"/>
+        <v>0.85</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30">
+        <v>25.5</v>
+      </c>
+      <c r="F30">
+        <v>0.21</v>
+      </c>
+      <c r="G30" s="16">
+        <f t="shared" si="0"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="16"/>
+        <v>2.5219999999999998</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="17"/>
+        <v>4.298</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="18"/>
+        <v>0.85</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="8">
+        <v>34</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="G31" s="15">
+        <f t="shared" si="0"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="16"/>
+        <v>1.6813333333333333</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="shared" si="17"/>
+        <v>2.8653333333333331</v>
+      </c>
+      <c r="J31" s="9">
+        <f t="shared" si="18"/>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>7.5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32">
+        <v>35</v>
+      </c>
+      <c r="F32">
+        <v>0.21</v>
+      </c>
+      <c r="G32" s="16">
+        <f t="shared" si="0"/>
+        <v>1.1904761904761905</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="16"/>
+        <v>1.6813333333333333</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="17"/>
+        <v>2.8653333333333331</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="18"/>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B25" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B6" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B4" r:id="rId12" display="https://www.edmundoptics.com/p/0179x-35mm-f-mount-titantl-telecentric-lens/38722/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B22" r:id="rId14" xr:uid="{9F3CB3DB-A9D8-4F4B-82A3-F2B7FF5C7500}"/>
-    <hyperlink ref="B20" r:id="rId15" xr:uid="{3E6CF2A1-EE83-4AA4-81AC-316DFC70DCB4}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B27" r:id="rId14" xr:uid="{9F3CB3DB-A9D8-4F4B-82A3-F2B7FF5C7500}"/>
+    <hyperlink ref="B22" r:id="rId15" xr:uid="{3E6CF2A1-EE83-4AA4-81AC-316DFC70DCB4}"/>
+    <hyperlink ref="B26" r:id="rId16" xr:uid="{83C8F5F9-4F41-4B79-9200-32A2609A2B5A}"/>
+    <hyperlink ref="B23" r:id="rId17" display="Plan Apo" xr:uid="{4A338276-1313-4961-8AB0-E02425183408}"/>
+    <hyperlink ref="B28" r:id="rId18" display="Plan Apo" xr:uid="{91EE068A-9052-4609-A361-89B25A613CAB}"/>
+    <hyperlink ref="B31" r:id="rId19" display="Plan Apo" xr:uid="{1DCE0DCD-261B-4BC5-B8A8-7141C7B15F4E}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{6E40E3E5-BEB2-4C03-A727-2595EFE56461}"/>
+    <hyperlink ref="B29" r:id="rId21" xr:uid="{7B8B86FD-0E4D-4B40-BE08-5FB6CFC7DD2D}"/>
+    <hyperlink ref="B30" r:id="rId22" display="Plan Apo" xr:uid="{8467164B-0D99-42AE-BE3B-C06EE6572BCC}"/>
+    <hyperlink ref="B32" r:id="rId23" xr:uid="{A49C9EA0-00B2-45B5-B328-8BB20A36800B}"/>
+    <hyperlink ref="B16" r:id="rId24" xr:uid="{6702FAF8-6190-4DF2-AC5D-679DF37144DA}"/>
+    <hyperlink ref="B9" r:id="rId25" xr:uid="{1AF3E83A-4010-402B-8196-B0C7E8688B12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>